<commit_message>
Bug Solved - Data Pengguna - Import Excel
</commit_message>
<xml_diff>
--- a/public/template_pengguna.xlsx
+++ b/public/template_pengguna.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Jenis Pengguna</t>
   </si>
@@ -35,16 +35,28 @@
     <t>Username</t>
   </si>
   <si>
+    <t>Nama Lengkap</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>UTP202401300001</t>
+    <t>ADM</t>
   </si>
   <si>
     <t>usersatu</t>
   </si>
   <si>
+    <t>User Satu</t>
+  </si>
+  <si>
+    <t>DSN</t>
+  </si>
+  <si>
     <t>userdua</t>
+  </si>
+  <si>
+    <t>User Dua</t>
   </si>
 </sst>
 </file>
@@ -988,20 +1000,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="18.4545454545455" customWidth="1"/>
     <col min="2" max="2" width="25.0909090909091" customWidth="1"/>
-    <col min="3" max="3" width="23.8181818181818" customWidth="1"/>
+    <col min="3" max="4" width="23.8181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,26 +1023,35 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>123456</v>
       </c>
     </row>

</xml_diff>